<commit_message>
check trung lap bien the khi import
</commit_message>
<xml_diff>
--- a/documents/BTSPTemple.xlsx
+++ b/documents/BTSPTemple.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>MÃ SP</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Trạng thái</t>
   </si>
   <si>
-    <t>Đỏ</t>
-  </si>
-  <si>
     <t>222.7</t>
   </si>
   <si>
@@ -55,6 +52,21 @@
   </si>
   <si>
     <t>100.3</t>
+  </si>
+  <si>
+    <t>Vàng</t>
+  </si>
+  <si>
+    <t>Trắng</t>
+  </si>
+  <si>
+    <t>Đen</t>
+  </si>
+  <si>
+    <t>Không hoạt động</t>
+  </si>
+  <si>
+    <t>Hồng</t>
   </si>
 </sst>
 </file>
@@ -372,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -386,7 +398,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -400,7 +412,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -411,25 +423,86 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>70</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
-        <v>7</v>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
export import excel, export qrcode by philong
</commit_message>
<xml_diff>
--- a/documents/BTSPTemple.xlsx
+++ b/documents/BTSPTemple.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>MÃ SP</t>
   </si>
@@ -48,9 +48,6 @@
     <t>nhập biến thể demo</t>
   </si>
   <si>
-    <t>SP0003</t>
-  </si>
-  <si>
     <t>100.3</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>Hồng</t>
+  </si>
+  <si>
+    <t>SP0004</t>
   </si>
 </sst>
 </file>
@@ -384,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -423,10 +423,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>70</v>
@@ -443,16 +443,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -463,41 +463,61 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update database table HoaDon
</commit_message>
<xml_diff>
--- a/documents/BTSPTemple.xlsx
+++ b/documents/BTSPTemple.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>MÃ SP</t>
   </si>
@@ -66,7 +66,7 @@
     <t>Hồng</t>
   </si>
   <si>
-    <t>SP0004</t>
+    <t>SP0006</t>
   </si>
 </sst>
 </file>
@@ -384,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -429,7 +429,7 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -498,26 +498,6 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>80</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Luong Ban Hang by Philong
</commit_message>
<xml_diff>
--- a/documents/BTSPTemple.xlsx
+++ b/documents/BTSPTemple.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>MÃ SP</t>
   </si>
@@ -66,7 +66,10 @@
     <t>Hồng</t>
   </si>
   <si>
-    <t>SP0006</t>
+    <t>SP0003</t>
+  </si>
+  <si>
+    <t>Demo</t>
   </si>
 </sst>
 </file>
@@ -384,16 +387,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="11.1796875" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -429,7 +432,7 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -498,6 +501,26 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>